<commit_message>
Store module has been added
</commit_message>
<xml_diff>
--- a/testData/Userdata.xlsx
+++ b/testData/Userdata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavan\restAssuredTraining\PetStoreAutomation\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyush ramteke\eclipse-workspace\E workplace\PetStoreAutomation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E65099-367B-4043-98C2-1CDC1656E877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6F0BFD-0517-4FD2-9588-B68D8C408F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="3146" windowWidth="22303" windowHeight="11974" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>UserID</t>
   </si>
@@ -91,13 +92,37 @@
   </si>
   <si>
     <t>Steve</t>
+  </si>
+  <si>
+    <t>userID</t>
+  </si>
+  <si>
+    <t>petID</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>shipDate</t>
+  </si>
+  <si>
+    <t>2023-12-06T04:03:05.234Z</t>
+  </si>
+  <si>
+    <t>placed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +147,28 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFA2FCA2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,7 +223,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,22 +514,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.23046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1010</v>
       </c>
@@ -520,7 +575,7 @@
         <v>1234567897</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1020</v>
       </c>
@@ -543,7 +598,7 @@
         <v>1234567897</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1030</v>
       </c>
@@ -571,4 +626,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55D328F-37A6-4B27-B5AB-A7F371B7B763}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5">
+        <v>122</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5">
+        <v>234</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5">
+        <v>222</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>